<commit_message>
Corrected PN of R12
</commit_message>
<xml_diff>
--- a/PCB/harp camera controller BOM.xlsx
+++ b/PCB/harp camera controller BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_camera_controller\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ABEEBAD-0B09-4C42-A082-3646BE589E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1926698C-30B7-45D8-9D19-7D3175F2F859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -531,9 +531,6 @@
     <t>CRCW04021K00FKEDC</t>
   </si>
   <si>
-    <t>RC0402FR-0740K2L</t>
-  </si>
-  <si>
     <t>ERJ-3EKF1000V</t>
   </si>
   <si>
@@ -562,6 +559,9 @@
   </si>
   <si>
     <t>EQUIVALENT: RCLAMP0504S.TCT</t>
+  </si>
+  <si>
+    <t>RC0402FR-0736K1L</t>
   </si>
 </sst>
 </file>
@@ -1142,11 +1142,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1515,7 +1515,7 @@
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1550,14 +1550,14 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -1579,7 +1579,7 @@
         <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>66</v>
       </c>
       <c r="G4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1625,7 +1625,7 @@
         <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1648,7 +1648,7 @@
         <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1671,7 +1671,7 @@
         <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1694,7 +1694,7 @@
         <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1717,7 +1717,7 @@
         <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1740,7 +1740,7 @@
         <v>67</v>
       </c>
       <c r="G10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1763,7 +1763,7 @@
         <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1786,7 +1786,7 @@
         <v>66</v>
       </c>
       <c r="G12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1809,7 +1809,7 @@
         <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1832,7 +1832,7 @@
         <v>66</v>
       </c>
       <c r="G14" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1855,7 +1855,7 @@
         <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1878,7 +1878,7 @@
         <v>66</v>
       </c>
       <c r="G16" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1901,7 +1901,7 @@
         <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
         <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1947,7 +1947,7 @@
         <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1970,7 +1970,7 @@
         <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1993,7 +1993,7 @@
         <v>66</v>
       </c>
       <c r="G21" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2016,7 +2016,7 @@
         <v>66</v>
       </c>
       <c r="G22" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2039,7 +2039,7 @@
         <v>67</v>
       </c>
       <c r="G23" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2062,7 +2062,7 @@
         <v>66</v>
       </c>
       <c r="G24" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2085,7 +2085,7 @@
         <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2108,7 +2108,7 @@
         <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2131,7 +2131,7 @@
         <v>66</v>
       </c>
       <c r="G27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2154,7 +2154,7 @@
         <v>66</v>
       </c>
       <c r="G28" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2177,7 +2177,7 @@
         <v>66</v>
       </c>
       <c r="G29" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2194,13 +2194,13 @@
         <v>138</v>
       </c>
       <c r="E30" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2223,7 +2223,7 @@
         <v>66</v>
       </c>
       <c r="G31" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2240,13 +2240,13 @@
         <v>140</v>
       </c>
       <c r="E32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
         <v>66</v>
       </c>
       <c r="G33" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -2286,13 +2286,13 @@
         <v>142</v>
       </c>
       <c r="E34" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G34" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -2309,13 +2309,13 @@
         <v>143</v>
       </c>
       <c r="E35" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G35" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2338,7 +2338,7 @@
         <v>66</v>
       </c>
       <c r="G36" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2361,7 +2361,7 @@
         <v>66</v>
       </c>
       <c r="G37" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2384,7 +2384,7 @@
         <v>66</v>
       </c>
       <c r="G38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
         <v>66</v>
       </c>
       <c r="G39" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2430,7 +2430,7 @@
         <v>66</v>
       </c>
       <c r="G40" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2452,19 +2452,19 @@
       <c r="F41" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G41" s="11" t="s">
-        <v>175</v>
+      <c r="G41" s="10" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="10"/>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
-      <c r="E42" s="10"/>
-      <c r="F42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
@@ -2511,14 +2511,14 @@
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+      <c r="A47" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11"/>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
@@ -2543,14 +2543,14 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
+      <c r="B50" s="11"/>
+      <c r="C50" s="11"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E51" s="7" t="s">

</xml_diff>

<commit_message>
Changed 5V output to 5.3V and released PCB v1.2
</commit_message>
<xml_diff>
--- a/PCB/harp camera controller BOM.xlsx
+++ b/PCB/harp camera controller BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_camera_controller\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1926698C-30B7-45D8-9D19-7D3175F2F859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD817E3C-8FC5-4DE6-981D-DEBE7139FCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'harp expander v1'!$A$43:$F$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'harp expander v1'!$A$44:$F$50</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="179">
   <si>
     <t>Qty</t>
   </si>
@@ -336,9 +336,6 @@
     <t>OSCILLATOR</t>
   </si>
   <si>
-    <t>31.6k</t>
-  </si>
-  <si>
     <t>RJ45</t>
   </si>
   <si>
@@ -444,9 +441,6 @@
     <t>R35</t>
   </si>
   <si>
-    <t>R2, R3, R4, R5, R6, R7, R8, R10, R11, R13, R15, R17, R21, R22, R23, R32, R33, R34, R36</t>
-  </si>
-  <si>
     <t>R14, R16, R24, R25, R28, R29</t>
   </si>
   <si>
@@ -561,7 +555,22 @@
     <t>EQUIVALENT: RCLAMP0504S.TCT</t>
   </si>
   <si>
-    <t>RC0402FR-0736K1L</t>
+    <t>34k 0.1%</t>
+  </si>
+  <si>
+    <t>ERA2AEB3402X</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R5, R6, R7, R8, R10, R11, R15, R17, R21, R22, R23, R32, R33, R34, R36</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>10k 0.1%</t>
+  </si>
+  <si>
+    <t>CPF0402B10KE1</t>
   </si>
 </sst>
 </file>
@@ -1512,10 +1521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1579,7 @@
         <v>45</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
         <v>44</v>
@@ -1579,7 +1588,7 @@
         <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1593,7 +1602,7 @@
         <v>78</v>
       </c>
       <c r="D4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
         <v>81</v>
@@ -1602,7 +1611,7 @@
         <v>66</v>
       </c>
       <c r="G4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1616,16 +1625,16 @@
         <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1639,16 +1648,16 @@
         <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1659,19 +1668,19 @@
         <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1685,7 +1694,7 @@
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
         <v>29</v>
@@ -1694,7 +1703,7 @@
         <v>66</v>
       </c>
       <c r="G8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1708,16 +1717,16 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1728,10 +1737,10 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E10" t="s">
         <v>31</v>
@@ -1740,7 +1749,7 @@
         <v>67</v>
       </c>
       <c r="G10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1754,16 +1763,16 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1777,7 +1786,7 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" t="s">
         <v>80</v>
@@ -1786,7 +1795,7 @@
         <v>66</v>
       </c>
       <c r="G12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1800,16 +1809,16 @@
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G13" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1823,7 +1832,7 @@
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
@@ -1832,7 +1841,7 @@
         <v>66</v>
       </c>
       <c r="G14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1846,16 +1855,16 @@
         <v>18</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1869,7 +1878,7 @@
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E16" t="s">
         <v>19</v>
@@ -1878,7 +1887,7 @@
         <v>66</v>
       </c>
       <c r="G16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1889,19 +1898,19 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1912,19 +1921,19 @@
         <v>95</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G18" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1938,16 +1947,16 @@
         <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1958,19 +1967,19 @@
         <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1984,7 +1993,7 @@
         <v>35</v>
       </c>
       <c r="D21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
         <v>36</v>
@@ -1993,7 +2002,7 @@
         <v>66</v>
       </c>
       <c r="G21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2004,19 +2013,19 @@
         <v>97</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
         <v>22</v>
       </c>
       <c r="E22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2030,7 +2039,7 @@
         <v>76</v>
       </c>
       <c r="D23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E23" t="s">
         <v>26</v>
@@ -2039,7 +2048,7 @@
         <v>67</v>
       </c>
       <c r="G23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2050,19 +2059,19 @@
         <v>98</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2079,13 +2088,13 @@
         <v>37</v>
       </c>
       <c r="E25" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>67</v>
       </c>
       <c r="G25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2099,7 +2108,7 @@
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E26" t="s">
         <v>74</v>
@@ -2108,7 +2117,7 @@
         <v>66</v>
       </c>
       <c r="G26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2122,21 +2131,21 @@
         <v>10</v>
       </c>
       <c r="D27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G27" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B28" t="s">
         <v>11</v>
@@ -2145,7 +2154,7 @@
         <v>10</v>
       </c>
       <c r="D28" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="E28" t="s">
         <v>12</v>
@@ -2154,76 +2163,76 @@
         <v>66</v>
       </c>
       <c r="G28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>13</v>
+        <v>177</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>137</v>
+        <v>176</v>
       </c>
       <c r="E29" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B30" t="s">
-        <v>100</v>
+        <v>13</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E30" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G30" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>173</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="E31" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2231,91 +2240,91 @@
         <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="E32" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E33" t="s">
-        <v>23</v>
+        <v>163</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G33" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>21</v>
       </c>
       <c r="D34" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
-        <v>166</v>
+        <v>23</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G34" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C35" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D35" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="E35" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -2323,22 +2332,22 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="E36" t="s">
-        <v>103</v>
+        <v>165</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2346,45 +2355,45 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>102</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>112</v>
       </c>
       <c r="D37" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E37" t="s">
-        <v>43</v>
+        <v>102</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G37" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E38" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G38" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -2392,45 +2401,45 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="C39" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D39" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="E39" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G39" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>47</v>
       </c>
       <c r="D40" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E40" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G40" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -2438,51 +2447,63 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C41" t="s">
+        <v>79</v>
+      </c>
+      <c r="D41" t="s">
+        <v>146</v>
+      </c>
+      <c r="E41" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G41" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
         <v>48</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>49</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D42" t="s">
         <v>50</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E42" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="F42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B42" s="11"/>
-      <c r="C42" s="11"/>
-      <c r="D42" s="11"/>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>56</v>
-      </c>
-      <c r="E43" t="s">
-        <v>68</v>
-      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E44" t="s">
         <v>68</v>
@@ -2493,121 +2514,132 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
+        <v>1</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
         <v>4</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>61</v>
       </c>
-      <c r="E46" s="4" t="s">
+      <c r="E47" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="1">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
-        <v>73</v>
-      </c>
-      <c r="E48" t="s">
-        <v>54</v>
-      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="11"/>
+      <c r="D48" s="11"/>
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>1</v>
       </c>
       <c r="D49" t="s">
+        <v>73</v>
+      </c>
+      <c r="E49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>1</v>
+      </c>
+      <c r="D50" t="s">
         <v>53</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E50" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E51" s="7" t="s">
+      <c r="B51" s="11"/>
+      <c r="C51" s="11"/>
+      <c r="D51" s="11"/>
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E52" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F52" s="8">
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E52" s="5" t="s">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E53" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F52" s="6">
+      <c r="F53" s="6">
         <v>34</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E53" s="7" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E54" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F53" s="8">
+      <c r="F54" s="8">
         <v>5</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
-        <v>64</v>
-      </c>
-      <c r="F54" s="1">
-        <v>101</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E55" t="s">
+        <v>64</v>
+      </c>
+      <c r="F55" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E56" t="s">
         <v>63</v>
       </c>
-      <c r="F55" s="1">
+      <c r="F56" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C56" s="9" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="9" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A42:F42"/>
-    <mergeCell ref="A50:F50"/>
-    <mergeCell ref="A47:F47"/>
+    <mergeCell ref="A43:F43"/>
+    <mergeCell ref="A51:F51"/>
+    <mergeCell ref="A48:F48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Replace some components out of stock.
</commit_message>
<xml_diff>
--- a/PCB/harp camera controller BOM.xlsx
+++ b/PCB/harp camera controller BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_camera_controller\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD817E3C-8FC5-4DE6-981D-DEBE7139FCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209CC13E-A87A-4984-8891-64F2DE05C3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'harp expander v1'!$A$44:$F$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'harp expander v1'!$A$45:$F$51</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="183">
   <si>
     <t>Qty</t>
   </si>
@@ -114,9 +114,6 @@
     <t>04025A470JAT2A</t>
   </si>
   <si>
-    <t>5690-111-100F</t>
-  </si>
-  <si>
     <t>BC850</t>
   </si>
   <si>
@@ -165,9 +162,6 @@
     <t>IC6</t>
   </si>
   <si>
-    <t>SI8610EC-B-IS</t>
-  </si>
-  <si>
     <t>SN74LVC1G125DBVT</t>
   </si>
   <si>
@@ -276,9 +270,6 @@
     <t>240-0002-1</t>
   </si>
   <si>
-    <t>C0402C331J5GACTU</t>
-  </si>
-  <si>
     <t>74HCT125D,653</t>
   </si>
   <si>
@@ -396,9 +387,6 @@
     <t>X3, X4, X5</t>
   </si>
   <si>
-    <t>C2, C4, C5, C6, C8, C9, C14, C15, C16, C18, C19, C20, C24, C25, C26, C27, C28, C29, C31, C33, C34, C36, C38</t>
-  </si>
-  <si>
     <t>C22, C30, C37</t>
   </si>
   <si>
@@ -483,24 +471,15 @@
     <t>SN74LVC1G240DBVR</t>
   </si>
   <si>
-    <t>ATXMEGA32A4U-AUR</t>
-  </si>
-  <si>
     <t>BLM18SG331TN1D</t>
   </si>
   <si>
-    <t>C1005X7R1H104K050BB</t>
-  </si>
-  <si>
     <t xml:space="preserve">885012205084  </t>
   </si>
   <si>
     <t>GCG188R91H184KA01D</t>
   </si>
   <si>
-    <t>CL21A475KLCLQNC</t>
-  </si>
-  <si>
     <t>T491D107K016AT7280</t>
   </si>
   <si>
@@ -513,21 +492,6 @@
     <t>IHLP2525CZER100M01</t>
   </si>
   <si>
-    <t>LT1765EFE#PBF</t>
-  </si>
-  <si>
-    <t>61300621121</t>
-  </si>
-  <si>
-    <t>CRCW040210R0FKEDC</t>
-  </si>
-  <si>
-    <t>CRCW04021K00FKEDC</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF1000V</t>
-  </si>
-  <si>
     <t>215877-1</t>
   </si>
   <si>
@@ -546,9 +510,6 @@
     <t>ALTERNATIVE: ADUM110N0BRZ</t>
   </si>
   <si>
-    <t>SIMILAR &amp; AVAILABLE = LP5951MFX-3.3/NOPB  &gt;&gt;  DIGIKEY_PN: 296-47807-2-ND   MOUSER_PN: 926-LP5951MFX33NOPB</t>
-  </si>
-  <si>
     <t>END OF LIFE COMPONENT BY SEPTEMBER 2021</t>
   </si>
   <si>
@@ -558,9 +519,6 @@
     <t>34k 0.1%</t>
   </si>
   <si>
-    <t>ERA2AEB3402X</t>
-  </si>
-  <si>
     <t>R2, R3, R4, R5, R6, R7, R8, R10, R11, R15, R17, R21, R22, R23, R32, R33, R34, R36</t>
   </si>
   <si>
@@ -571,6 +529,60 @@
   </si>
   <si>
     <t>CPF0402B10KE1</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C2, C5, C6, C8, C9, C14, C15, C16, C18, C19, C20, C24, C25, C26, C27, C28, C29, C31, C33, C34, C36, C38</t>
+  </si>
+  <si>
+    <t>100nF 50V</t>
+  </si>
+  <si>
+    <t>CGA2B3X7R1H104K050BB</t>
+  </si>
+  <si>
+    <t>GRM155R71E104KE14D</t>
+  </si>
+  <si>
+    <t>C0402C331J5GAC7867</t>
+  </si>
+  <si>
+    <t>GRM21BR61H475KE51L</t>
+  </si>
+  <si>
+    <t>569-0111-100F</t>
+  </si>
+  <si>
+    <t>LT1765EFE#TRPBF</t>
+  </si>
+  <si>
+    <t>67996-206HLF</t>
+  </si>
+  <si>
+    <t>ERJ-PA2J100X</t>
+  </si>
+  <si>
+    <t>ERJ-2RKF1001X</t>
+  </si>
+  <si>
+    <t>RT0402BRD0734KL</t>
+  </si>
+  <si>
+    <t>RCS0402100RFKED</t>
+  </si>
+  <si>
+    <t>CMDSH-3 TR PBFREE</t>
+  </si>
+  <si>
+    <t>SI8610EC-B-ISR</t>
+  </si>
+  <si>
+    <t>LP5951MFX-3.3/NOPB</t>
+  </si>
+  <si>
+    <t>ATXMEGA32A4U-A</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1142,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1141,10 +1153,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1521,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,40 +1563,40 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
+      <c r="A2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G3" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1596,22 +1604,22 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>111</v>
+      </c>
+      <c r="E4" t="s">
         <v>78</v>
       </c>
-      <c r="D4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" t="s">
-        <v>81</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1619,22 +1627,22 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G5" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1642,22 +1650,22 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1665,22 +1673,22 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1688,22 +1696,22 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" t="s">
         <v>28</v>
       </c>
-      <c r="D8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" t="s">
-        <v>29</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1711,22 +1719,22 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1734,27 +1742,27 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>104</v>
-      </c>
-      <c r="D10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G10" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -1763,154 +1771,154 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>166</v>
       </c>
       <c r="E11" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G11" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>167</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>165</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>168</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>170</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G13" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C14" t="s">
         <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>146</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G14" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="E15" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
         <v>18</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>147</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G16" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="D17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E17" t="s">
-        <v>154</v>
+        <v>19</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G17" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1918,22 +1926,22 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D18" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="E18" t="s">
+        <v>171</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" t="s">
         <v>155</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G18" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1941,22 +1949,22 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C19" t="s">
-        <v>75</v>
+        <v>103</v>
       </c>
       <c r="D19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="E19" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G19" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1964,22 +1972,22 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
-        <v>107</v>
+        <v>73</v>
       </c>
       <c r="D20" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E20" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G20" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1987,22 +1995,22 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2010,68 +2018,68 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>97</v>
+        <v>33</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>22</v>
+        <v>126</v>
       </c>
       <c r="E22" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G22" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>105</v>
       </c>
       <c r="D23" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>151</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G23" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="E24" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2079,22 +2087,22 @@
         <v>1</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>95</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>106</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>128</v>
       </c>
       <c r="E25" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G25" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2102,22 +2110,22 @@
         <v>1</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>38</v>
       </c>
       <c r="C26" t="s">
-        <v>38</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
-        <v>133</v>
+        <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>174</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G26" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2125,137 +2133,137 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="D27" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="E27" t="s">
-        <v>161</v>
+        <v>72</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G27" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
         <v>10</v>
       </c>
       <c r="D28" t="s">
+        <v>130</v>
+      </c>
+      <c r="E28" t="s">
         <v>175</v>
       </c>
-      <c r="E28" t="s">
-        <v>12</v>
-      </c>
       <c r="F28" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G28" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B29" t="s">
-        <v>177</v>
+        <v>11</v>
       </c>
       <c r="C29" t="s">
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E29" t="s">
-        <v>178</v>
+        <v>12</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G29" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>163</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="E30" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G30" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>173</v>
+        <v>13</v>
       </c>
       <c r="C31" t="s">
         <v>10</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="E31" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G31" t="s">
-        <v>167</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>14</v>
+        <v>160</v>
       </c>
       <c r="C32" t="s">
         <v>10</v>
       </c>
       <c r="D32" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>177</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G32" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -2263,91 +2271,91 @@
         <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
-        <v>163</v>
+        <v>15</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G33" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="E34" t="s">
-        <v>23</v>
+        <v>178</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G34" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>20</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="D35" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="E35" t="s">
-        <v>164</v>
+        <v>23</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G35" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C36" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E36" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G36" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -2355,22 +2363,22 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E37" t="s">
-        <v>102</v>
+        <v>153</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G37" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -2378,45 +2386,45 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C38" t="s">
-        <v>41</v>
+        <v>109</v>
       </c>
       <c r="D38" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>179</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G38" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D39" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="E39" t="s">
-        <v>33</v>
+        <v>180</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G39" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -2424,45 +2432,42 @@
         <v>2</v>
       </c>
       <c r="B40" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C40" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D40" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="E40" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G40" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="D41" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="E41" t="s">
-        <v>52</v>
+        <v>181</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G41" t="s">
-        <v>171</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -2470,54 +2475,66 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" t="s">
+        <v>50</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G42" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" t="s">
         <v>48</v>
       </c>
-      <c r="C42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D42" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" t="s">
-        <v>48</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="11"/>
-      <c r="C43" s="11"/>
-      <c r="D43" s="11"/>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
+      <c r="E43" t="s">
+        <v>46</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G43" s="8" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
-        <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>56</v>
-      </c>
-      <c r="E44" t="s">
-        <v>68</v>
-      </c>
+      <c r="A44" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E45" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -2525,121 +2542,132 @@
         <v>1</v>
       </c>
       <c r="D46" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E46" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
+        <v>1</v>
+      </c>
+      <c r="D47" t="s">
+        <v>56</v>
+      </c>
+      <c r="E47" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
         <v>4</v>
       </c>
-      <c r="D47" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="D48" t="s">
+        <v>59</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="1">
-        <v>1</v>
-      </c>
-      <c r="D49" t="s">
-        <v>73</v>
-      </c>
-      <c r="E49" t="s">
-        <v>54</v>
-      </c>
+      <c r="A49" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>1</v>
       </c>
       <c r="D50" t="s">
+        <v>71</v>
+      </c>
+      <c r="E50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>1</v>
+      </c>
+      <c r="D51" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" t="s">
         <v>53</v>
       </c>
-      <c r="E50" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
-      <c r="D51" s="11"/>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E52" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F52" s="8">
-        <v>39</v>
-      </c>
+      <c r="A52" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E53" s="5" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="F53" s="6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E54" t="s">
+        <v>83</v>
+      </c>
+      <c r="F54" s="1">
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E54" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="F54" s="8">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E55" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F55" s="6">
         <v>5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E55" t="s">
-        <v>64</v>
-      </c>
-      <c r="F55" s="1">
-        <v>101</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F56" s="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
+        <v>61</v>
+      </c>
+      <c r="F57" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C57" s="9" t="s">
-        <v>88</v>
-      </c>
-    </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
-        <v>89</v>
+      <c r="C58" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A43:F43"/>
-    <mergeCell ref="A51:F51"/>
-    <mergeCell ref="A48:F48"/>
+    <mergeCell ref="A44:F44"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A49:F49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed R8 from BOM (doesn't exist on schematic).
</commit_message>
<xml_diff>
--- a/PCB/harp camera controller BOM.xlsx
+++ b/PCB/harp camera controller BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEPS\Documents\github\harp-tech\harp_camera_controller\PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209CC13E-A87A-4984-8891-64F2DE05C3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593E02F7-500A-41BB-83DD-D32FC7719C1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="harp expander v1" sheetId="1" r:id="rId1"/>
@@ -519,9 +519,6 @@
     <t>34k 0.1%</t>
   </si>
   <si>
-    <t>R2, R3, R4, R5, R6, R7, R8, R10, R11, R15, R17, R21, R22, R23, R32, R33, R34, R36</t>
-  </si>
-  <si>
     <t>R13</t>
   </si>
   <si>
@@ -583,6 +580,9 @@
   </si>
   <si>
     <t>ATXMEGA32A4U-A</t>
+  </si>
+  <si>
+    <t>R2, R3, R4, R5, R6, R7, R10, R11, R15, R17, R21, R22, R23, R32, R33, R34, R36</t>
   </si>
 </sst>
 </file>
@@ -1531,8 +1531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1682,7 +1682,7 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>64</v>
@@ -1771,10 +1771,10 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E11" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>64</v>
@@ -1788,16 +1788,16 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>64</v>
@@ -1820,7 +1820,7 @@
         <v>117</v>
       </c>
       <c r="E13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>64</v>
@@ -1935,7 +1935,7 @@
         <v>122</v>
       </c>
       <c r="E18" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>64</v>
@@ -2073,7 +2073,7 @@
         <v>127</v>
       </c>
       <c r="E24" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>65</v>
@@ -2096,7 +2096,7 @@
         <v>128</v>
       </c>
       <c r="E25" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>64</v>
@@ -2119,7 +2119,7 @@
         <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>65</v>
@@ -2165,7 +2165,7 @@
         <v>130</v>
       </c>
       <c r="E28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>64</v>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>11</v>
@@ -2185,7 +2185,7 @@
         <v>10</v>
       </c>
       <c r="D29" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="E29" t="s">
         <v>12</v>
@@ -2202,16 +2202,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C30" t="s">
         <v>10</v>
       </c>
       <c r="D30" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>64</v>
@@ -2234,7 +2234,7 @@
         <v>131</v>
       </c>
       <c r="E31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>64</v>
@@ -2257,7 +2257,7 @@
         <v>132</v>
       </c>
       <c r="E32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>64</v>
@@ -2303,7 +2303,7 @@
         <v>134</v>
       </c>
       <c r="E34" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>64</v>
@@ -2395,7 +2395,7 @@
         <v>138</v>
       </c>
       <c r="E38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>64</v>
@@ -2418,7 +2418,7 @@
         <v>139</v>
       </c>
       <c r="E39" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>64</v>
@@ -2464,7 +2464,7 @@
         <v>141</v>
       </c>
       <c r="E41" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>64</v>

</xml_diff>